<commit_message>
update info of dahei
</commit_message>
<xml_diff>
--- a/UCATS/pages/猫咪档案.xlsx
+++ b/UCATS/pages/猫咪档案.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C46E77-F3DA-41FB-BB7C-A4FF23323BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5957CEF-24D8-45A8-A86C-494C4EDF57A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="校内喵" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="203">
   <si>
     <t>ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -620,9 +620,6 @@
   </si>
   <si>
     <t>疑似菜菜 格力高 憨八嘎的兄弟</t>
-  </si>
-  <si>
-    <t>大黑被送到救助站，随时接受领养</t>
   </si>
   <si>
     <t>2022年11月01号</t>
@@ -1353,27 +1350,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1396,6 +1372,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1699,9 +1696,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD597"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T12" sqref="T12"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="111" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="12" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T44" sqref="T44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
@@ -1761,21 +1758,21 @@
       <c r="A3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="63"/>
+      <c r="C3" s="56"/>
       <c r="D3" s="2"/>
-      <c r="F3" s="59" t="s">
+      <c r="F3" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="69"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="64" t="s">
+      <c r="J3" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="65"/>
+      <c r="K3" s="58"/>
       <c r="L3" s="4"/>
       <c r="M3" s="13" t="s">
         <v>20</v>
@@ -1799,7 +1796,7 @@
       <c r="U3" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="V3" s="57" t="s">
+      <c r="V3" s="65" t="s">
         <v>36</v>
       </c>
       <c r="W3" s="7" t="s">
@@ -1840,7 +1837,7 @@
       <c r="U4" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="V4" s="58"/>
+      <c r="V4" s="66"/>
       <c r="Y4" s="23" t="s">
         <v>52</v>
       </c>
@@ -1849,18 +1846,18 @@
       </c>
     </row>
     <row r="5" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="68"/>
-      <c r="H5" s="62" t="s">
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="61"/>
+      <c r="H5" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="63"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="56"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
@@ -1876,7 +1873,7 @@
       <c r="U5" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="V5" s="58"/>
+      <c r="V5" s="66"/>
       <c r="Y5" s="3"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.15">
@@ -1891,7 +1888,7 @@
       <c r="U6" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="V6" s="58" t="s">
+      <c r="V6" s="66" t="s">
         <v>37</v>
       </c>
       <c r="W6" s="7" t="s">
@@ -1939,7 +1936,7 @@
       <c r="U7" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="V7" s="58"/>
+      <c r="V7" s="66"/>
       <c r="Y7" s="21">
         <v>2</v>
       </c>
@@ -1969,7 +1966,7 @@
       <c r="U8" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="V8" s="58" t="s">
+      <c r="V8" s="66" t="s">
         <v>38</v>
       </c>
       <c r="Y8" s="21">
@@ -2001,7 +1998,7 @@
       <c r="U9" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="V9" s="58"/>
+      <c r="V9" s="66"/>
       <c r="Y9" s="21">
         <v>4</v>
       </c>
@@ -2024,7 +2021,7 @@
       </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
-      <c r="Q10" s="55" t="s">
+      <c r="Q10" s="63" t="s">
         <v>73</v>
       </c>
       <c r="R10" s="31" t="s">
@@ -2059,7 +2056,7 @@
       </c>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
-      <c r="Q11" s="56"/>
+      <c r="Q11" s="64"/>
       <c r="R11" s="4"/>
       <c r="V11" s="34" t="s">
         <v>76</v>
@@ -2107,7 +2104,7 @@
         <v>40</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O12" s="3" t="s">
         <v>9</v>
@@ -2182,7 +2179,7 @@
         <v>0</v>
       </c>
       <c r="O13" s="39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P13" s="43">
         <v>2</v>
@@ -2190,7 +2187,7 @@
       <c r="Q13" s="44"/>
       <c r="R13" s="43"/>
       <c r="S13" s="39" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="T13" s="39"/>
       <c r="U13" s="38"/>
@@ -2242,7 +2239,7 @@
         <v>0</v>
       </c>
       <c r="O14" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="P14" s="43">
         <v>6</v>
@@ -2250,10 +2247,10 @@
       <c r="Q14" s="44"/>
       <c r="R14" s="43"/>
       <c r="S14" s="39" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="T14" s="39" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="U14" s="38"/>
       <c r="V14" s="38"/>
@@ -2300,7 +2297,7 @@
         <v>0</v>
       </c>
       <c r="O15" s="39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P15" s="38">
         <v>-1</v>
@@ -2308,7 +2305,7 @@
       <c r="Q15" s="44"/>
       <c r="R15" s="43"/>
       <c r="S15" s="39" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T15" s="39"/>
       <c r="U15" s="38"/>
@@ -2345,7 +2342,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K16" s="38">
         <v>0</v>
@@ -2356,7 +2353,7 @@
         <v>0</v>
       </c>
       <c r="O16" s="39" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="P16" s="38">
         <v>0</v>
@@ -2364,10 +2361,10 @@
       <c r="Q16" s="44"/>
       <c r="R16" s="43"/>
       <c r="S16" s="39" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="T16" s="39" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="U16" s="38"/>
       <c r="V16" s="38"/>
@@ -2414,7 +2411,7 @@
         <v>0</v>
       </c>
       <c r="O17" s="39" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="P17" s="47">
         <v>6</v>
@@ -2422,7 +2419,7 @@
       <c r="Q17" s="44"/>
       <c r="R17" s="43"/>
       <c r="S17" s="39" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="T17" s="39"/>
       <c r="U17" s="38"/>
@@ -2472,7 +2469,7 @@
         <v>0</v>
       </c>
       <c r="O18" s="39" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P18" s="47">
         <v>6</v>
@@ -2480,12 +2477,12 @@
       <c r="Q18" s="44"/>
       <c r="R18" s="43"/>
       <c r="S18" s="39" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="T18" s="39"/>
       <c r="U18" s="38"/>
       <c r="V18" s="38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="W18" s="38"/>
       <c r="X18" s="38"/>
@@ -2538,7 +2535,7 @@
       <c r="Q19" s="43"/>
       <c r="R19" s="43"/>
       <c r="S19" s="39" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="T19" s="39"/>
       <c r="U19" s="43"/>
@@ -2575,7 +2572,7 @@
         <v>0</v>
       </c>
       <c r="J20" s="39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K20" s="38">
         <v>0</v>
@@ -2594,7 +2591,7 @@
       <c r="Q20" s="43"/>
       <c r="R20" s="43"/>
       <c r="S20" s="39" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="T20" s="39"/>
       <c r="U20" s="43"/>
@@ -2650,7 +2647,7 @@
       <c r="Q21" s="43"/>
       <c r="R21" s="43"/>
       <c r="S21" s="39" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="T21" s="39"/>
       <c r="U21" s="43"/>
@@ -2697,14 +2694,14 @@
         <v>1</v>
       </c>
       <c r="L22" s="43" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M22" s="43"/>
       <c r="N22" s="42">
         <v>0</v>
       </c>
       <c r="O22" s="39" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P22" s="43">
         <v>6</v>
@@ -2712,10 +2709,10 @@
       <c r="Q22" s="43"/>
       <c r="R22" s="43"/>
       <c r="S22" s="39" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="T22" s="39" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="U22" s="43"/>
       <c r="V22" s="38" t="s">
@@ -2764,7 +2761,7 @@
         <v>0</v>
       </c>
       <c r="O23" s="39" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="P23" s="43">
         <v>0</v>
@@ -2772,7 +2769,7 @@
       <c r="Q23" s="43"/>
       <c r="R23" s="43"/>
       <c r="S23" s="39" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="T23" s="39"/>
       <c r="U23" s="43"/>
@@ -2815,7 +2812,7 @@
         <v>1</v>
       </c>
       <c r="L24" s="43" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M24" s="50">
         <v>44713</v>
@@ -2824,7 +2821,7 @@
         <v>0</v>
       </c>
       <c r="O24" s="39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="P24" s="43">
         <v>6</v>
@@ -2832,7 +2829,7 @@
       <c r="Q24" s="43"/>
       <c r="R24" s="43"/>
       <c r="S24" s="39" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T24" s="39"/>
       <c r="U24" s="43"/>
@@ -2882,7 +2879,7 @@
         <v>1</v>
       </c>
       <c r="O25" s="39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P25" s="43">
         <v>6</v>
@@ -2890,7 +2887,7 @@
       <c r="Q25" s="43"/>
       <c r="R25" s="43"/>
       <c r="S25" s="51" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="T25" s="51"/>
       <c r="U25" s="43"/>
@@ -2946,7 +2943,7 @@
       <c r="Q26" s="43"/>
       <c r="R26" s="43"/>
       <c r="S26" s="51" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="T26" s="39"/>
       <c r="U26" s="43"/>
@@ -3004,7 +3001,7 @@
       <c r="Q27" s="43"/>
       <c r="R27" s="43"/>
       <c r="S27" s="51" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="T27" s="39"/>
       <c r="U27" s="43"/>
@@ -3108,7 +3105,7 @@
         <v>0</v>
       </c>
       <c r="O29" s="39" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="P29" s="43">
         <v>6</v>
@@ -3116,7 +3113,7 @@
       <c r="Q29" s="43"/>
       <c r="R29" s="43"/>
       <c r="S29" s="39" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="T29" s="39"/>
       <c r="U29" s="43"/>
@@ -3164,7 +3161,7 @@
         <v>0</v>
       </c>
       <c r="O30" s="39" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="P30" s="43">
         <v>6</v>
@@ -3172,7 +3169,7 @@
       <c r="Q30" s="43"/>
       <c r="R30" s="43"/>
       <c r="S30" s="39" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="T30" s="39"/>
       <c r="U30" s="43"/>
@@ -3228,7 +3225,7 @@
       <c r="Q31" s="43"/>
       <c r="R31" s="43"/>
       <c r="S31" s="39" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="T31" s="39"/>
       <c r="U31" s="43"/>
@@ -3248,26 +3245,26 @@
         <v>20</v>
       </c>
       <c r="C32" s="39" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D32" s="38">
         <v>1</v>
       </c>
       <c r="E32" s="43"/>
       <c r="F32" s="43" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G32" s="43">
         <v>2</v>
       </c>
       <c r="H32" s="39" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I32" s="46">
         <v>-1</v>
       </c>
       <c r="J32" s="39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K32" s="38">
         <v>-1</v>
@@ -3278,7 +3275,7 @@
         <v>0</v>
       </c>
       <c r="O32" s="39" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="P32" s="43">
         <v>0</v>
@@ -3286,7 +3283,7 @@
       <c r="Q32" s="43"/>
       <c r="R32" s="43"/>
       <c r="S32" s="39" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="T32" s="39"/>
       <c r="U32" s="43"/>
@@ -3304,14 +3301,14 @@
         <v>21</v>
       </c>
       <c r="C33" s="39" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D33" s="38">
         <v>0</v>
       </c>
       <c r="E33" s="43"/>
       <c r="F33" s="43" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G33" s="43">
         <v>2</v>
@@ -3323,7 +3320,7 @@
         <v>-1</v>
       </c>
       <c r="J33" s="39" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K33" s="38">
         <v>-1</v>
@@ -3334,7 +3331,7 @@
         <v>0</v>
       </c>
       <c r="O33" s="39" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P33" s="43">
         <v>0</v>
@@ -3377,7 +3374,7 @@
         <v>-1</v>
       </c>
       <c r="J34" s="39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K34" s="38">
         <v>-1</v>
@@ -3388,7 +3385,7 @@
         <v>0</v>
       </c>
       <c r="O34" s="39" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="P34" s="43">
         <v>-1</v>
@@ -3431,7 +3428,7 @@
         <v>-1</v>
       </c>
       <c r="J35" s="39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K35" s="38">
         <v>-1</v>
@@ -3442,7 +3439,7 @@
         <v>0</v>
       </c>
       <c r="O35" s="39" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P35" s="43">
         <v>-1</v>
@@ -3496,7 +3493,7 @@
         <v>0</v>
       </c>
       <c r="O36" s="39" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="P36" s="43">
         <v>6</v>
@@ -3507,7 +3504,7 @@
       <c r="T36" s="39"/>
       <c r="U36" s="43"/>
       <c r="V36" s="43" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="W36" s="43"/>
       <c r="X36" s="43"/>
@@ -3552,7 +3549,7 @@
         <v>0</v>
       </c>
       <c r="O37" s="39" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="P37" s="43">
         <v>6</v>
@@ -3563,7 +3560,7 @@
       <c r="T37" s="39"/>
       <c r="U37" s="43"/>
       <c r="V37" s="43" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="W37" s="43"/>
       <c r="X37" s="43"/>
@@ -3657,7 +3654,7 @@
         <v>1</v>
       </c>
       <c r="L39" s="43" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M39" s="43"/>
       <c r="N39" s="42">
@@ -3675,7 +3672,7 @@
       <c r="T39" s="39"/>
       <c r="U39" s="43"/>
       <c r="V39" s="43" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="W39" s="43"/>
       <c r="X39" s="43"/>
@@ -3733,7 +3730,7 @@
       <c r="T40" s="39"/>
       <c r="U40" s="43"/>
       <c r="V40" s="43" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="W40" s="43"/>
       <c r="X40" s="43"/>
@@ -3754,7 +3751,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="43" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F41" s="43" t="s">
         <v>124</v>
@@ -3791,7 +3788,7 @@
       <c r="T41" s="39"/>
       <c r="U41" s="43"/>
       <c r="V41" s="43" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="W41" s="43"/>
       <c r="X41" s="43"/>
@@ -3836,7 +3833,7 @@
         <v>0</v>
       </c>
       <c r="O42" s="39" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P42" s="43">
         <v>6</v>
@@ -3890,7 +3887,7 @@
         <v>0</v>
       </c>
       <c r="O43" s="39" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="P43" s="43">
         <v>0</v>
@@ -3944,7 +3941,7 @@
         <v>0</v>
       </c>
       <c r="O44" s="39" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P44" s="43">
         <v>5</v>
@@ -3952,9 +3949,7 @@
       <c r="Q44" s="43"/>
       <c r="R44" s="43"/>
       <c r="S44" s="43"/>
-      <c r="T44" s="39" t="s">
-        <v>148</v>
-      </c>
+      <c r="T44" s="39"/>
       <c r="U44" s="43"/>
       <c r="V44" s="43"/>
       <c r="W44" s="43"/>
@@ -6724,15 +6719,15 @@
   </sheetData>
   <autoFilter ref="A12:U114" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="9">
+    <mergeCell ref="V3:V5"/>
+    <mergeCell ref="V6:V7"/>
+    <mergeCell ref="V8:V9"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="H5:K5"/>
     <mergeCell ref="Q10:Q11"/>
-    <mergeCell ref="V3:V5"/>
-    <mergeCell ref="V6:V7"/>
-    <mergeCell ref="V8:V9"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>